<commit_message>
Muistion kirjauksia ja pohjan luontia, kaavion lisäys, ajankäyttön päivitys IK
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB4B0FE-5FD0-4F81-8456-989D6BF3DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DB2406-1A54-4D1F-8A1D-3EB49C246338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>Ohjelman muokkausta</t>
+  </si>
+  <si>
+    <t>15.2.2024</t>
+  </si>
+  <si>
+    <t>Palaveri/review</t>
+  </si>
+  <si>
+    <t>Palaveri/review, UML, kirjauksia</t>
+  </si>
+  <si>
+    <t>11.2.2024</t>
+  </si>
+  <si>
+    <t>UML perehtyminen/aloittaminen</t>
   </si>
 </sst>
 </file>
@@ -103,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d\.m\.yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="d\.m\.yyyy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -258,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -303,34 +318,43 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -645,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,9 +923,15 @@
       <c r="J7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="31"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="13"/>
+      <c r="M7" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="7">
+        <v>2</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="R7" s="34">
         <v>45328</v>
       </c>
@@ -945,9 +975,15 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="37"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="13"/>
+      <c r="C9" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="H9" s="29">
         <v>45331</v>
       </c>
@@ -974,9 +1010,15 @@
       <c r="C10" s="37"/>
       <c r="D10" s="5"/>
       <c r="E10" s="13"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="13"/>
+      <c r="H10" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="M10" s="31"/>
       <c r="N10" s="7"/>
       <c r="O10" s="13"/>
@@ -994,15 +1036,27 @@
       <c r="C11" s="37"/>
       <c r="D11" s="5"/>
       <c r="E11" s="13"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="13"/>
+      <c r="H11" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3">
+        <v>5</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="M11" s="31"/>
       <c r="N11" s="7"/>
       <c r="O11" s="13"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="13"/>
+      <c r="R11" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="S11" s="9">
+        <v>2</v>
+      </c>
+      <c r="T11" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="37"/>
@@ -1088,7 +1142,7 @@
       <c r="S17" s="9"/>
       <c r="T17" s="13"/>
     </row>
-    <row r="18" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37"/>
       <c r="D18" s="5"/>
       <c r="E18" s="13"/>
@@ -1102,7 +1156,7 @@
       <c r="S18" s="9"/>
       <c r="T18" s="13"/>
     </row>
-    <row r="19" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37"/>
       <c r="D19" s="5"/>
       <c r="E19" s="13"/>
@@ -1116,7 +1170,7 @@
       <c r="S19" s="9"/>
       <c r="T19" s="13"/>
     </row>
-    <row r="20" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37"/>
       <c r="D20" s="5"/>
       <c r="E20" s="13"/>
@@ -1130,7 +1184,7 @@
       <c r="S20" s="9"/>
       <c r="T20" s="13"/>
     </row>
-    <row r="21" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37"/>
       <c r="D21" s="5"/>
       <c r="E21" s="13"/>
@@ -1144,7 +1198,7 @@
       <c r="S21" s="9"/>
       <c r="T21" s="13"/>
     </row>
-    <row r="22" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37"/>
       <c r="D22" s="5"/>
       <c r="E22" s="13"/>
@@ -1158,7 +1212,7 @@
       <c r="S22" s="9"/>
       <c r="T22" s="13"/>
     </row>
-    <row r="23" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37"/>
       <c r="D23" s="5"/>
       <c r="E23" s="13"/>
@@ -1172,7 +1226,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="13"/>
     </row>
-    <row r="24" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37"/>
       <c r="D24" s="5"/>
       <c r="E24" s="13"/>
@@ -1186,34 +1240,118 @@
       <c r="S24" s="9"/>
       <c r="T24" s="13"/>
     </row>
-    <row r="25" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>14</v>
-      </c>
+    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37"/>
-      <c r="D25" s="6">
-        <f>SUM(D3:D24)</f>
-        <v>18</v>
-      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="13"/>
       <c r="H25" s="29"/>
-      <c r="I25" s="4">
-        <f>SUM(I3:I23)</f>
-        <v>24</v>
-      </c>
+      <c r="I25" s="3"/>
       <c r="J25" s="13"/>
       <c r="M25" s="31"/>
-      <c r="N25" s="8">
-        <f>SUM(N3:N23)</f>
-        <v>13</v>
-      </c>
+      <c r="N25" s="7"/>
       <c r="O25" s="13"/>
       <c r="R25" s="34"/>
-      <c r="S25" s="10">
-        <f>SUM(S3:S23)</f>
-        <v>30</v>
-      </c>
+      <c r="S25" s="9"/>
       <c r="T25" s="13"/>
+    </row>
+    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="37"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="13"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="13"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="13"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="13"/>
+    </row>
+    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="37"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="13"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="13"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="13"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="13"/>
+    </row>
+    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="37"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="13"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="13"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="13"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="13"/>
+    </row>
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="37"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="13"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="13"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="13"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="13"/>
+    </row>
+    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="37"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="13"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="13"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="13"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="13"/>
+    </row>
+    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="37"/>
+      <c r="D31" s="6">
+        <f>SUM(D3:D30)</f>
+        <v>20</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="4">
+        <f>SUM(I3:I29)</f>
+        <v>31</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="8">
+        <f>SUM(N3:N29)</f>
+        <v>15</v>
+      </c>
+      <c r="O31" s="13"/>
+      <c r="R31" s="34"/>
+      <c r="S31" s="10">
+        <f>SUM(S3:S29)</f>
+        <v>32</v>
+      </c>
+      <c r="T31" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Poistettiin vanha ohjelmisto ja lisättiin uusi ohjelmisto jota ruvetaan työstämään -Jiska
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DB2406-1A54-4D1F-8A1D-3EB49C246338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97375A69-7941-4014-9B44-0F3435F3007C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>UML perehtyminen/aloittaminen</t>
+  </si>
+  <si>
+    <t>Ohjelmiston kehittämistä</t>
   </si>
 </sst>
 </file>
@@ -373,9 +376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 -teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -413,7 +416,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -519,7 +522,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -661,7 +664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,9 +964,15 @@
       <c r="J8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="13"/>
+      <c r="M8" s="31">
+        <v>45338</v>
+      </c>
+      <c r="N8" s="7">
+        <v>4</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="R8" s="34">
         <v>45331</v>
       </c>
@@ -1343,7 +1352,7 @@
       <c r="M31" s="31"/>
       <c r="N31" s="8">
         <f>SUM(N3:N29)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="O31" s="13"/>
       <c r="R31" s="34"/>
@@ -1359,9 +1368,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1509,19 +1521,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1545,9 +1553,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Retro ja 2. sprintin aloitus palaveri -IK
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97375A69-7941-4014-9B44-0F3435F3007C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AE8407-1EE3-401A-B30F-FECF47FB3F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Ohjelmiston kehittämistä</t>
+  </si>
+  <si>
+    <t>GitHubin korjailua</t>
+  </si>
+  <si>
+    <t>16.2.2024</t>
+  </si>
+  <si>
+    <t>Retro</t>
+  </si>
+  <si>
+    <t>13.2.2024</t>
   </si>
 </sst>
 </file>
@@ -276,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -330,25 +342,21 @@
     <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -356,6 +364,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -376,9 +387,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 -teema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -416,7 +427,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -522,7 +533,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -664,7 +675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -672,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +758,7 @@
       <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="32">
         <v>45314</v>
       </c>
       <c r="D3" s="17">
@@ -783,7 +794,7 @@
       <c r="Q3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="32">
+      <c r="R3" s="30">
         <v>45314</v>
       </c>
       <c r="S3" s="20">
@@ -794,7 +805,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="35">
+      <c r="C4" s="32">
         <v>45321</v>
       </c>
       <c r="D4" s="17">
@@ -821,7 +832,7 @@
       <c r="O4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="32">
+      <c r="R4" s="30">
         <v>45321</v>
       </c>
       <c r="S4" s="20">
@@ -832,7 +843,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="36">
+      <c r="C5" s="33">
         <v>45323</v>
       </c>
       <c r="D5" s="5">
@@ -850,7 +861,7 @@
       <c r="J5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="29">
         <v>45323</v>
       </c>
       <c r="N5" s="7">
@@ -859,7 +870,7 @@
       <c r="O5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="33">
+      <c r="R5" s="31">
         <v>45323</v>
       </c>
       <c r="S5" s="9">
@@ -870,7 +881,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="37">
+      <c r="C6" s="33">
         <v>45327</v>
       </c>
       <c r="D6" s="5">
@@ -888,7 +899,7 @@
       <c r="J6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="35">
         <v>45325</v>
       </c>
       <c r="N6" s="7">
@@ -897,18 +908,18 @@
       <c r="O6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="34">
+      <c r="R6" s="36">
         <v>45324</v>
       </c>
       <c r="S6" s="9">
         <v>3</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="37">
+      <c r="C7" s="33">
         <v>45328</v>
       </c>
       <c r="D7" s="5">
@@ -917,7 +928,7 @@
       <c r="E7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="34">
         <v>45328</v>
       </c>
       <c r="I7" s="3">
@@ -926,7 +937,7 @@
       <c r="J7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="35" t="s">
         <v>20</v>
       </c>
       <c r="N7" s="7">
@@ -935,7 +946,7 @@
       <c r="O7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="R7" s="34">
+      <c r="R7" s="36">
         <v>45328</v>
       </c>
       <c r="S7" s="9">
@@ -946,7 +957,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="37">
+      <c r="C8" s="33">
         <v>45331</v>
       </c>
       <c r="D8" s="5">
@@ -955,7 +966,7 @@
       <c r="E8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="34">
         <v>45328</v>
       </c>
       <c r="I8" s="3">
@@ -964,7 +975,7 @@
       <c r="J8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="35">
         <v>45338</v>
       </c>
       <c r="N8" s="7">
@@ -973,7 +984,7 @@
       <c r="O8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="34">
+      <c r="R8" s="36">
         <v>45331</v>
       </c>
       <c r="S8" s="9">
@@ -984,7 +995,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="5">
@@ -993,7 +1004,7 @@
       <c r="E9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="34">
         <v>45331</v>
       </c>
       <c r="I9" s="3">
@@ -1002,10 +1013,16 @@
       <c r="J9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="31"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="13"/>
-      <c r="R9" s="34">
+      <c r="M9" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="7">
+        <v>2</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="36">
         <v>45333</v>
       </c>
       <c r="S9" s="9">
@@ -1016,10 +1033,16 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="37"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="13"/>
-      <c r="H10" s="38" t="s">
+      <c r="C10" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="34" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="3">
@@ -1028,10 +1051,10 @@
       <c r="J10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="31"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="7"/>
       <c r="O10" s="13"/>
-      <c r="R10" s="34">
+      <c r="R10" s="36">
         <v>45334</v>
       </c>
       <c r="S10" s="9">
@@ -1042,294 +1065,318 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="37"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="5"/>
       <c r="E11" s="13"/>
-      <c r="H11" s="38" t="s">
-        <v>20</v>
+      <c r="H11" s="34" t="s">
+        <v>29</v>
       </c>
       <c r="I11" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="31"/>
+        <v>16</v>
+      </c>
+      <c r="M11" s="35"/>
       <c r="N11" s="7"/>
       <c r="O11" s="13"/>
-      <c r="R11" s="40" t="s">
-        <v>20</v>
+      <c r="R11" s="36" t="s">
+        <v>29</v>
       </c>
       <c r="S11" s="9">
         <v>2</v>
       </c>
       <c r="T11" s="21" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="37"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="5"/>
       <c r="E12" s="13"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="13"/>
-      <c r="M12" s="31"/>
+      <c r="H12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3">
+        <v>5</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="35"/>
       <c r="N12" s="7"/>
       <c r="O12" s="13"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="13"/>
+      <c r="R12" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12" s="9">
+        <v>2</v>
+      </c>
+      <c r="T12" s="21" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="37"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="5"/>
       <c r="E13" s="13"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="13"/>
-      <c r="M13" s="31"/>
+      <c r="H13" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="35"/>
       <c r="N13" s="7"/>
       <c r="O13" s="13"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="13"/>
+      <c r="R13" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="9">
+        <v>2</v>
+      </c>
+      <c r="T13" s="21" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="37"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="5"/>
       <c r="E14" s="13"/>
-      <c r="H14" s="29"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="3"/>
       <c r="J14" s="13"/>
-      <c r="M14" s="31"/>
+      <c r="M14" s="35"/>
       <c r="N14" s="7"/>
       <c r="O14" s="13"/>
-      <c r="R14" s="34"/>
+      <c r="R14" s="36"/>
       <c r="S14" s="9"/>
       <c r="T14" s="13"/>
     </row>
     <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="37"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="5"/>
       <c r="E15" s="13"/>
-      <c r="H15" s="29"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="3"/>
       <c r="J15" s="13"/>
-      <c r="M15" s="31"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="7"/>
       <c r="O15" s="13"/>
-      <c r="R15" s="34"/>
+      <c r="R15" s="36"/>
       <c r="S15" s="9"/>
       <c r="T15" s="13"/>
     </row>
     <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="37"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="5"/>
       <c r="E16" s="13"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="3"/>
       <c r="J16" s="13"/>
-      <c r="M16" s="31"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="7"/>
       <c r="O16" s="13"/>
-      <c r="R16" s="34"/>
+      <c r="R16" s="36"/>
       <c r="S16" s="9"/>
       <c r="T16" s="13"/>
     </row>
     <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="37"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="5"/>
       <c r="E17" s="13"/>
-      <c r="H17" s="29"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="3"/>
       <c r="J17" s="13"/>
-      <c r="M17" s="31"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="7"/>
       <c r="O17" s="13"/>
-      <c r="R17" s="34"/>
+      <c r="R17" s="36"/>
       <c r="S17" s="9"/>
       <c r="T17" s="13"/>
     </row>
     <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="37"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="5"/>
       <c r="E18" s="13"/>
-      <c r="H18" s="29"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="3"/>
       <c r="J18" s="13"/>
-      <c r="M18" s="31"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="7"/>
       <c r="O18" s="13"/>
-      <c r="R18" s="34"/>
+      <c r="R18" s="36"/>
       <c r="S18" s="9"/>
       <c r="T18" s="13"/>
     </row>
     <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="37"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="5"/>
       <c r="E19" s="13"/>
-      <c r="H19" s="29"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="3"/>
       <c r="J19" s="13"/>
-      <c r="M19" s="31"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="7"/>
       <c r="O19" s="13"/>
-      <c r="R19" s="34"/>
+      <c r="R19" s="36"/>
       <c r="S19" s="9"/>
       <c r="T19" s="13"/>
     </row>
     <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="37"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="5"/>
       <c r="E20" s="13"/>
-      <c r="H20" s="29"/>
+      <c r="H20" s="34"/>
       <c r="I20" s="3"/>
       <c r="J20" s="13"/>
-      <c r="M20" s="31"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="7"/>
       <c r="O20" s="13"/>
-      <c r="R20" s="34"/>
+      <c r="R20" s="36"/>
       <c r="S20" s="9"/>
       <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="37"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="5"/>
       <c r="E21" s="13"/>
-      <c r="H21" s="29"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="3"/>
       <c r="J21" s="13"/>
-      <c r="M21" s="31"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="7"/>
       <c r="O21" s="13"/>
-      <c r="R21" s="34"/>
+      <c r="R21" s="36"/>
       <c r="S21" s="9"/>
       <c r="T21" s="13"/>
     </row>
     <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="37"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="5"/>
       <c r="E22" s="13"/>
-      <c r="H22" s="29"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="3"/>
       <c r="J22" s="13"/>
-      <c r="M22" s="31"/>
+      <c r="M22" s="35"/>
       <c r="N22" s="7"/>
       <c r="O22" s="13"/>
-      <c r="R22" s="34"/>
+      <c r="R22" s="36"/>
       <c r="S22" s="9"/>
       <c r="T22" s="13"/>
     </row>
     <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="37"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="5"/>
       <c r="E23" s="13"/>
-      <c r="H23" s="29"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="3"/>
       <c r="J23" s="13"/>
-      <c r="M23" s="31"/>
+      <c r="M23" s="35"/>
       <c r="N23" s="7"/>
       <c r="O23" s="13"/>
-      <c r="R23" s="34"/>
+      <c r="R23" s="36"/>
       <c r="S23" s="9"/>
       <c r="T23" s="13"/>
     </row>
     <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="37"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="5"/>
       <c r="E24" s="13"/>
-      <c r="H24" s="29"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="3"/>
       <c r="J24" s="13"/>
-      <c r="M24" s="31"/>
+      <c r="M24" s="35"/>
       <c r="N24" s="7"/>
       <c r="O24" s="13"/>
-      <c r="R24" s="34"/>
+      <c r="R24" s="36"/>
       <c r="S24" s="9"/>
       <c r="T24" s="13"/>
     </row>
     <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="37"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="5"/>
       <c r="E25" s="13"/>
-      <c r="H25" s="29"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="3"/>
       <c r="J25" s="13"/>
-      <c r="M25" s="31"/>
+      <c r="M25" s="35"/>
       <c r="N25" s="7"/>
       <c r="O25" s="13"/>
-      <c r="R25" s="34"/>
+      <c r="R25" s="36"/>
       <c r="S25" s="9"/>
       <c r="T25" s="13"/>
     </row>
     <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="37"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="5"/>
       <c r="E26" s="13"/>
-      <c r="H26" s="29"/>
+      <c r="H26" s="34"/>
       <c r="I26" s="3"/>
       <c r="J26" s="13"/>
-      <c r="M26" s="31"/>
+      <c r="M26" s="35"/>
       <c r="N26" s="7"/>
       <c r="O26" s="13"/>
-      <c r="R26" s="34"/>
+      <c r="R26" s="36"/>
       <c r="S26" s="9"/>
       <c r="T26" s="13"/>
     </row>
     <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="37"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="5"/>
       <c r="E27" s="13"/>
-      <c r="H27" s="29"/>
+      <c r="H27" s="34"/>
       <c r="I27" s="3"/>
       <c r="J27" s="13"/>
-      <c r="M27" s="31"/>
+      <c r="M27" s="35"/>
       <c r="N27" s="7"/>
       <c r="O27" s="13"/>
-      <c r="R27" s="34"/>
+      <c r="R27" s="36"/>
       <c r="S27" s="9"/>
       <c r="T27" s="13"/>
     </row>
     <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="37"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="5"/>
       <c r="E28" s="13"/>
-      <c r="H28" s="29"/>
+      <c r="H28" s="34"/>
       <c r="I28" s="3"/>
       <c r="J28" s="13"/>
-      <c r="M28" s="31"/>
+      <c r="M28" s="35"/>
       <c r="N28" s="7"/>
       <c r="O28" s="13"/>
-      <c r="R28" s="34"/>
+      <c r="R28" s="36"/>
       <c r="S28" s="9"/>
       <c r="T28" s="13"/>
     </row>
     <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="37"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="5"/>
       <c r="E29" s="13"/>
-      <c r="H29" s="29"/>
+      <c r="H29" s="34"/>
       <c r="I29" s="3"/>
       <c r="J29" s="13"/>
-      <c r="M29" s="31"/>
+      <c r="M29" s="35"/>
       <c r="N29" s="7"/>
       <c r="O29" s="13"/>
-      <c r="R29" s="34"/>
+      <c r="R29" s="36"/>
       <c r="S29" s="9"/>
       <c r="T29" s="13"/>
     </row>
     <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="37"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="5"/>
       <c r="E30" s="13"/>
-      <c r="H30" s="29"/>
+      <c r="H30" s="34"/>
       <c r="I30" s="3"/>
       <c r="J30" s="13"/>
-      <c r="M30" s="31"/>
+      <c r="M30" s="35"/>
       <c r="N30" s="7"/>
       <c r="O30" s="13"/>
-      <c r="R30" s="34"/>
+      <c r="R30" s="36"/>
       <c r="S30" s="9"/>
       <c r="T30" s="13"/>
     </row>
@@ -1337,30 +1384,43 @@
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="37"/>
+      <c r="C31" s="33"/>
       <c r="D31" s="6">
         <f>SUM(D3:D30)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E31" s="13"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="4">
-        <f>SUM(I3:I29)</f>
-        <v>31</v>
-      </c>
+      <c r="H31" s="34"/>
+      <c r="I31" s="3"/>
       <c r="J31" s="13"/>
-      <c r="M31" s="31"/>
+      <c r="M31" s="35"/>
       <c r="N31" s="8">
         <f>SUM(N3:N29)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O31" s="13"/>
-      <c r="R31" s="34"/>
-      <c r="S31" s="10">
-        <f>SUM(S3:S29)</f>
-        <v>32</v>
-      </c>
+      <c r="R31" s="36"/>
+      <c r="S31" s="9"/>
       <c r="T31" s="13"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C32" s="37"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="4">
+        <f>SUM(I3:I30)</f>
+        <v>35</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="10">
+        <f>SUM(S3:S30)</f>
+        <v>36</v>
+      </c>
+      <c r="T32" s="13"/>
+    </row>
+    <row r="33" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H33" s="37"/>
+      <c r="R33" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pientä säätöä ohjelmassa sekä tuntikirjaukset -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0E7BA3-278A-4FA3-9459-E2F0F9A8F067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD71E92-6337-4399-94C4-D2974172BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Jsonin lisäys ohjelmaan ja mallikonsolin tekeminen</t>
+  </si>
+  <si>
+    <t>Ohjelmiston kehittämistä ja toiminnalisuuksien luonti</t>
+  </si>
+  <si>
+    <t>Ohjelmiston kehittämistä, luokat/failsafet</t>
   </si>
 </sst>
 </file>
@@ -706,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="R8" s="36">
         <v>45331</v>
@@ -1079,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="R10" s="36">
         <v>45334</v>
@@ -1110,9 +1116,15 @@
       <c r="J11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="35"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="13"/>
+      <c r="M11" s="35">
+        <v>45342</v>
+      </c>
+      <c r="N11" s="7">
+        <v>1</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="R11" s="36" t="s">
         <v>29</v>
       </c>
@@ -1142,9 +1154,15 @@
       <c r="J12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="35"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="13"/>
+      <c r="M12" s="35">
+        <v>45344</v>
+      </c>
+      <c r="N12" s="7">
+        <v>1</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="R12" s="36" t="s">
         <v>20</v>
       </c>
@@ -1465,7 +1483,7 @@
       <c r="M31" s="35"/>
       <c r="N31" s="8">
         <f>SUM(N3:N29)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O31" s="13"/>
       <c r="R31" s="36"/>

</xml_diff>

<commit_message>
Vaatimusmäärittelyä ja tuntikirjaus -ET
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eve\Documents\Hamk\ohjelmistoprojekti\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0E7BA3-278A-4FA3-9459-E2F0F9A8F067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C600D90-696B-4501-A831-58D3CFD02FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -707,7 +707,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1162,7 @@
       <c r="D13" s="5">
         <v>2</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="21" t="s">
         <v>32</v>
       </c>
       <c r="H13" s="34" t="s">
@@ -1194,7 +1194,7 @@
       <c r="D14" s="5">
         <v>2</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="21" t="s">
         <v>33</v>
       </c>
       <c r="H14" s="34">
@@ -1214,9 +1214,15 @@
       <c r="T14" s="13"/>
     </row>
     <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="33"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="13"/>
+      <c r="C15" s="33">
+        <v>45344</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="H15" s="34">
         <v>45343</v>
       </c>
@@ -1456,7 +1462,7 @@
       <c r="C31" s="33"/>
       <c r="D31" s="6">
         <f>SUM(D3:D30)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E31" s="13"/>
       <c r="H31" s="34"/>
@@ -1497,12 +1503,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1650,15 +1653,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1682,10 +1689,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Vaatimusmäärityksen, muistiinpanojen ja tuntipäiväkirjan päivittäminen -KV
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eve\Documents\Hamk\ohjelmistoprojekti\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lahde\OneDrive\Tiedostot\Gitit\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C600D90-696B-4501-A831-58D3CFD02FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C58A9B-CB0A-4BF7-BB72-37EA59D322CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>Jsonin lisäys ohjelmaan ja mallikonsolin tekeminen</t>
+  </si>
+  <si>
+    <t>Vaatimusmäärittelyn tekemistä</t>
+  </si>
+  <si>
+    <t>Vaatimusmäärittelyn tekemistä ja Sprintin kirjaamista</t>
+  </si>
+  <si>
+    <t>Scrumiin tutustuminen, käsikirjan ja vaatimusmäärittelyn lukemista</t>
   </si>
 </sst>
 </file>
@@ -706,38 +715,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="K10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="49.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="25.140625" customWidth="1"/>
-    <col min="20" max="20" width="51.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="10" max="10" width="52.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" customWidth="1"/>
+    <col min="15" max="15" width="49.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="25.109375" customWidth="1"/>
+    <col min="20" max="20" width="51.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
@@ -775,7 +784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
@@ -825,7 +834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="32">
         <v>45321</v>
       </c>
@@ -863,7 +872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="33">
         <v>45323</v>
       </c>
@@ -901,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="33">
         <v>45327</v>
       </c>
@@ -939,7 +948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="33">
         <v>45328</v>
       </c>
@@ -977,7 +986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="33">
         <v>45331</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="33">
         <v>45334</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="33">
         <v>45336</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="33" t="s">
         <v>20</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="33" t="s">
         <v>27</v>
       </c>
@@ -1155,7 +1164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="33">
         <v>45339</v>
       </c>
@@ -1187,7 +1196,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="33">
         <v>45343</v>
       </c>
@@ -1209,11 +1218,17 @@
       <c r="M14" s="35"/>
       <c r="N14" s="7"/>
       <c r="O14" s="13"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="13"/>
-    </row>
-    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R14" s="36">
+        <v>45340</v>
+      </c>
+      <c r="S14" s="9">
+        <v>2</v>
+      </c>
+      <c r="T14" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="33">
         <v>45344</v>
       </c>
@@ -1235,11 +1250,17 @@
       <c r="M15" s="35"/>
       <c r="N15" s="7"/>
       <c r="O15" s="13"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="13"/>
-    </row>
-    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R15" s="36">
+        <v>45342</v>
+      </c>
+      <c r="S15" s="9">
+        <v>1</v>
+      </c>
+      <c r="T15" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="33"/>
       <c r="D16" s="5"/>
       <c r="E16" s="13"/>
@@ -1255,11 +1276,17 @@
       <c r="M16" s="35"/>
       <c r="N16" s="7"/>
       <c r="O16" s="13"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="13"/>
-    </row>
-    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R16" s="36">
+        <v>45344</v>
+      </c>
+      <c r="S16" s="9">
+        <v>4</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="33"/>
       <c r="D17" s="5"/>
       <c r="E17" s="13"/>
@@ -1269,11 +1296,17 @@
       <c r="M17" s="35"/>
       <c r="N17" s="7"/>
       <c r="O17" s="13"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="13"/>
-    </row>
-    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="36">
+        <v>45345</v>
+      </c>
+      <c r="S17" s="9">
+        <v>4</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="33"/>
       <c r="D18" s="5"/>
       <c r="E18" s="13"/>
@@ -1287,7 +1320,7 @@
       <c r="S18" s="9"/>
       <c r="T18" s="13"/>
     </row>
-    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="33"/>
       <c r="D19" s="5"/>
       <c r="E19" s="13"/>
@@ -1301,7 +1334,7 @@
       <c r="S19" s="9"/>
       <c r="T19" s="13"/>
     </row>
-    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="33"/>
       <c r="D20" s="5"/>
       <c r="E20" s="13"/>
@@ -1315,7 +1348,7 @@
       <c r="S20" s="9"/>
       <c r="T20" s="13"/>
     </row>
-    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="33"/>
       <c r="D21" s="5"/>
       <c r="E21" s="13"/>
@@ -1329,7 +1362,7 @@
       <c r="S21" s="9"/>
       <c r="T21" s="13"/>
     </row>
-    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="33"/>
       <c r="D22" s="5"/>
       <c r="E22" s="13"/>
@@ -1343,7 +1376,7 @@
       <c r="S22" s="9"/>
       <c r="T22" s="13"/>
     </row>
-    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="33"/>
       <c r="D23" s="5"/>
       <c r="E23" s="13"/>
@@ -1357,7 +1390,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="13"/>
     </row>
-    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="33"/>
       <c r="D24" s="5"/>
       <c r="E24" s="13"/>
@@ -1371,7 +1404,7 @@
       <c r="S24" s="9"/>
       <c r="T24" s="13"/>
     </row>
-    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="33"/>
       <c r="D25" s="5"/>
       <c r="E25" s="13"/>
@@ -1385,7 +1418,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="13"/>
     </row>
-    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="33"/>
       <c r="D26" s="5"/>
       <c r="E26" s="13"/>
@@ -1399,7 +1432,7 @@
       <c r="S26" s="9"/>
       <c r="T26" s="13"/>
     </row>
-    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="33"/>
       <c r="D27" s="5"/>
       <c r="E27" s="13"/>
@@ -1413,7 +1446,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="13"/>
     </row>
-    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="33"/>
       <c r="D28" s="5"/>
       <c r="E28" s="13"/>
@@ -1427,7 +1460,7 @@
       <c r="S28" s="9"/>
       <c r="T28" s="13"/>
     </row>
-    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="33"/>
       <c r="D29" s="5"/>
       <c r="E29" s="13"/>
@@ -1441,7 +1474,7 @@
       <c r="S29" s="9"/>
       <c r="T29" s="13"/>
     </row>
-    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="33"/>
       <c r="D30" s="5"/>
       <c r="E30" s="13"/>
@@ -1455,7 +1488,7 @@
       <c r="S30" s="9"/>
       <c r="T30" s="13"/>
     </row>
-    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1511,7 @@
       <c r="S31" s="9"/>
       <c r="T31" s="13"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C32" s="37"/>
       <c r="H32" s="34"/>
       <c r="I32" s="4">
@@ -1489,11 +1522,11 @@
       <c r="R32" s="36"/>
       <c r="S32" s="10">
         <f>SUM(S3:S30)</f>
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="T32" s="13"/>
     </row>
-    <row r="33" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H33" s="37"/>
       <c r="R33" s="37"/>
     </row>
@@ -1503,9 +1536,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1653,19 +1689,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1689,9 +1721,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UML ja ajankäytön päivitys
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lahde\OneDrive\Tiedostot\Gitit\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eve\Documents\Hamk\ohjelmistoprojekti\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD4B767-F322-461D-B995-E7F48CCD33FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A71BB8D-506E-465A-A981-EF44F9034AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Tutustuminen ULM-mallinnukseen</t>
+  </si>
+  <si>
+    <t>UML:n ja ohjelmistokoodiin tutustuminen</t>
   </si>
 </sst>
 </file>
@@ -718,38 +721,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="49.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" customWidth="1"/>
-    <col min="10" max="10" width="52.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-    <col min="14" max="14" width="27.44140625" customWidth="1"/>
-    <col min="15" max="15" width="49.5546875" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="19" width="25.109375" customWidth="1"/>
-    <col min="20" max="20" width="51.33203125" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="52.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="27.42578125" customWidth="1"/>
+    <col min="15" max="15" width="49.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="19" max="19" width="25.140625" customWidth="1"/>
+    <col min="20" max="20" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
@@ -787,7 +790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
@@ -837,7 +840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="32">
         <v>45321</v>
       </c>
@@ -875,7 +878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="33">
         <v>45323</v>
       </c>
@@ -913,7 +916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="33">
         <v>45327</v>
       </c>
@@ -951,7 +954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="33">
         <v>45328</v>
       </c>
@@ -989,7 +992,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="33">
         <v>45331</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="33">
         <v>45334</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="33">
         <v>45336</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="33" t="s">
         <v>20</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="33" t="s">
         <v>27</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="33">
         <v>45339</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="33">
         <v>45343</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="33">
         <v>45344</v>
       </c>
@@ -1263,10 +1266,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="33"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="13"/>
+    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="33">
+        <v>45345</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>28</v>
+      </c>
       <c r="H16" s="34">
         <v>45344</v>
       </c>
@@ -1289,10 +1298,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="33"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="13"/>
+    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="33">
+        <v>45347</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="H17" s="34"/>
       <c r="I17" s="3"/>
       <c r="J17" s="21"/>
@@ -1309,7 +1324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="33"/>
       <c r="D18" s="5"/>
       <c r="E18" s="13"/>
@@ -1329,7 +1344,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="33"/>
       <c r="D19" s="5"/>
       <c r="E19" s="13"/>
@@ -1349,7 +1364,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="33"/>
       <c r="D20" s="5"/>
       <c r="E20" s="13"/>
@@ -1363,7 +1378,7 @@
       <c r="S20" s="9"/>
       <c r="T20" s="13"/>
     </row>
-    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="33"/>
       <c r="D21" s="5"/>
       <c r="E21" s="13"/>
@@ -1377,7 +1392,7 @@
       <c r="S21" s="9"/>
       <c r="T21" s="13"/>
     </row>
-    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="33"/>
       <c r="D22" s="5"/>
       <c r="E22" s="13"/>
@@ -1391,7 +1406,7 @@
       <c r="S22" s="9"/>
       <c r="T22" s="13"/>
     </row>
-    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="33"/>
       <c r="D23" s="5"/>
       <c r="E23" s="13"/>
@@ -1405,7 +1420,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="13"/>
     </row>
-    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="33"/>
       <c r="D24" s="5"/>
       <c r="E24" s="13"/>
@@ -1419,7 +1434,7 @@
       <c r="S24" s="9"/>
       <c r="T24" s="13"/>
     </row>
-    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="33"/>
       <c r="D25" s="5"/>
       <c r="E25" s="13"/>
@@ -1433,7 +1448,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="13"/>
     </row>
-    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="33"/>
       <c r="D26" s="5"/>
       <c r="E26" s="13"/>
@@ -1447,7 +1462,7 @@
       <c r="S26" s="9"/>
       <c r="T26" s="13"/>
     </row>
-    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="33"/>
       <c r="D27" s="5"/>
       <c r="E27" s="13"/>
@@ -1461,7 +1476,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="13"/>
     </row>
-    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="33"/>
       <c r="D28" s="5"/>
       <c r="E28" s="13"/>
@@ -1475,7 +1490,7 @@
       <c r="S28" s="9"/>
       <c r="T28" s="13"/>
     </row>
-    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="33"/>
       <c r="D29" s="5"/>
       <c r="E29" s="13"/>
@@ -1489,7 +1504,7 @@
       <c r="S29" s="9"/>
       <c r="T29" s="13"/>
     </row>
-    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="33"/>
       <c r="D30" s="5"/>
       <c r="E30" s="13"/>
@@ -1503,14 +1518,14 @@
       <c r="S30" s="9"/>
       <c r="T30" s="13"/>
     </row>
-    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="6">
         <f>SUM(D3:D30)</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E31" s="13"/>
       <c r="H31" s="34"/>
@@ -1526,7 +1541,7 @@
       <c r="S31" s="9"/>
       <c r="T31" s="13"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32" s="37"/>
       <c r="H32" s="34"/>
       <c r="I32" s="4">
@@ -1541,7 +1556,7 @@
       </c>
       <c r="T32" s="13"/>
     </row>
-    <row r="33" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H33" s="37"/>
       <c r="R33" s="37"/>
     </row>
@@ -1551,12 +1566,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1704,15 +1716,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1736,10 +1752,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Muokattiin ampumataulukkotoimintoa ja se tallennusmetodeja -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55B2D3E-92A1-4B46-A283-00B6E2F65795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D7C504-E408-443C-A380-4A7748075E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Xaml-puolen kehittämistä</t>
+  </si>
+  <si>
+    <t>Ohjelmiston kehittämistä/Xaml</t>
   </si>
 </sst>
 </file>
@@ -725,7 +728,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1210,7 +1213,7 @@
       <c r="N13" s="7">
         <v>1</v>
       </c>
-      <c r="O13" s="13" t="s">
+      <c r="O13" s="21" t="s">
         <v>40</v>
       </c>
       <c r="R13" s="36" t="s">
@@ -1248,7 +1251,7 @@
       <c r="N14" s="7">
         <v>2</v>
       </c>
-      <c r="O14" s="13" t="s">
+      <c r="O14" s="21" t="s">
         <v>42</v>
       </c>
       <c r="R14" s="36">
@@ -1280,9 +1283,15 @@
       <c r="J15" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="35"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="13"/>
+      <c r="M15" s="35">
+        <v>45349</v>
+      </c>
+      <c r="N15" s="7">
+        <v>4</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>43</v>
+      </c>
       <c r="R15" s="36">
         <v>45342</v>
       </c>
@@ -1561,7 +1570,7 @@
       <c r="M31" s="35"/>
       <c r="N31" s="8">
         <f>SUM(N3:N29)</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="O31" s="13"/>
       <c r="R31" s="36"/>
@@ -1593,9 +1602,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1743,19 +1755,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1779,9 +1787,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Saatiin toiminnallisuus ja tietokulkemaan ikkunoiden välillä -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D7C504-E408-443C-A380-4A7748075E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7EC5BF-D1E7-43C9-8837-41DD805E7D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -728,7 +728,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1321,9 +1321,15 @@
       <c r="J16" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="M16" s="35"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="13"/>
+      <c r="M16" s="35">
+        <v>45350</v>
+      </c>
+      <c r="N16" s="7">
+        <v>5</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>43</v>
+      </c>
       <c r="R16" s="36">
         <v>45344</v>
       </c>
@@ -1570,7 +1576,7 @@
       <c r="M31" s="35"/>
       <c r="N31" s="8">
         <f>SUM(N3:N29)</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="O31" s="13"/>
       <c r="R31" s="36"/>
@@ -1602,12 +1608,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1755,15 +1758,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1787,10 +1794,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lisättiin Tulosten tarkasteluun toimintoja -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3B51AE-0616-40D0-B305-9FE51289CFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EE1E1D-DF62-4EE5-83F9-B6D46114AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>xaml/Kello, ulkoasua, perehtymistä</t>
+  </si>
+  <si>
+    <t>Ohjelmiston Kehittämistä/Xaml</t>
   </si>
 </sst>
 </file>
@@ -734,7 +737,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1397,9 +1400,15 @@
       <c r="J18" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="35"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="13"/>
+      <c r="M18" s="35">
+        <v>45352</v>
+      </c>
+      <c r="N18" s="7">
+        <v>3</v>
+      </c>
+      <c r="O18" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="R18" s="36">
         <v>45345</v>
       </c>
@@ -1606,7 +1615,7 @@
       <c r="M31" s="35"/>
       <c r="N31" s="8">
         <f>SUM(N3:N29)</f>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="O31" s="13"/>
       <c r="R31" s="36"/>
@@ -1638,9 +1647,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1788,19 +1800,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1824,9 +1832,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Palaverimuistio ja tuntiseuranta -ET
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eve\Documents\Hamk\ohjelmistoprojekti\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EE1E1D-DF62-4EE5-83F9-B6D46114AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A494A8-97AB-41B2-8870-3985255AA7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Ohjelmiston Kehittämistä/Xaml</t>
+  </si>
+  <si>
+    <t>Koodin kehittämistä / Xaml</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -737,37 +740,37 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="49.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" customWidth="1"/>
-    <col min="10" max="10" width="52.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-    <col min="14" max="14" width="27.44140625" customWidth="1"/>
-    <col min="15" max="15" width="49.5546875" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="19" width="25.109375" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="52.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="27.42578125" customWidth="1"/>
+    <col min="15" max="15" width="49.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="19" max="19" width="25.140625" customWidth="1"/>
     <col min="20" max="20" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
@@ -805,7 +808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
@@ -855,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="32">
         <v>45321</v>
       </c>
@@ -893,7 +896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="33">
         <v>45323</v>
       </c>
@@ -931,7 +934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="33">
         <v>45327</v>
       </c>
@@ -969,7 +972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="33">
         <v>45328</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="33">
         <v>45331</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="33">
         <v>45334</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="33">
         <v>45336</v>
       </c>
@@ -1121,7 +1124,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="33" t="s">
         <v>20</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="33" t="s">
         <v>27</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="33">
         <v>45339</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="33">
         <v>45343</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="33">
         <v>45344</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="33">
         <v>45345</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="33">
         <v>45347</v>
       </c>
@@ -1387,10 +1390,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="33"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="13"/>
+    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="33">
+        <v>45348</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>47</v>
+      </c>
       <c r="H18" s="34">
         <v>45348</v>
       </c>
@@ -1419,10 +1428,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="33"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="13"/>
+    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="33">
+        <v>45352</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>28</v>
+      </c>
       <c r="H19" s="34">
         <v>45350</v>
       </c>
@@ -1445,7 +1460,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="33"/>
       <c r="D20" s="5"/>
       <c r="E20" s="13"/>
@@ -1459,7 +1474,7 @@
       <c r="S20" s="9"/>
       <c r="T20" s="13"/>
     </row>
-    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="33"/>
       <c r="D21" s="5"/>
       <c r="E21" s="13"/>
@@ -1473,7 +1488,7 @@
       <c r="S21" s="9"/>
       <c r="T21" s="13"/>
     </row>
-    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="33"/>
       <c r="D22" s="5"/>
       <c r="E22" s="13"/>
@@ -1487,7 +1502,7 @@
       <c r="S22" s="9"/>
       <c r="T22" s="13"/>
     </row>
-    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="33"/>
       <c r="D23" s="5"/>
       <c r="E23" s="13"/>
@@ -1501,7 +1516,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="13"/>
     </row>
-    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="33"/>
       <c r="D24" s="5"/>
       <c r="E24" s="13"/>
@@ -1515,7 +1530,7 @@
       <c r="S24" s="9"/>
       <c r="T24" s="13"/>
     </row>
-    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="33"/>
       <c r="D25" s="5"/>
       <c r="E25" s="13"/>
@@ -1529,7 +1544,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="13"/>
     </row>
-    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="33"/>
       <c r="D26" s="5"/>
       <c r="E26" s="13"/>
@@ -1543,7 +1558,7 @@
       <c r="S26" s="9"/>
       <c r="T26" s="13"/>
     </row>
-    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="33"/>
       <c r="D27" s="5"/>
       <c r="E27" s="13"/>
@@ -1557,7 +1572,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="13"/>
     </row>
-    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="33"/>
       <c r="D28" s="5"/>
       <c r="E28" s="13"/>
@@ -1571,7 +1586,7 @@
       <c r="S28" s="9"/>
       <c r="T28" s="13"/>
     </row>
-    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="33"/>
       <c r="D29" s="5"/>
       <c r="E29" s="13"/>
@@ -1585,7 +1600,7 @@
       <c r="S29" s="9"/>
       <c r="T29" s="13"/>
     </row>
-    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="33"/>
       <c r="D30" s="5"/>
       <c r="E30" s="13"/>
@@ -1599,14 +1614,14 @@
       <c r="S30" s="9"/>
       <c r="T30" s="13"/>
     </row>
-    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="6">
         <f>SUM(D3:D30)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E31" s="13"/>
       <c r="H31" s="34"/>
@@ -1622,7 +1637,7 @@
       <c r="S31" s="9"/>
       <c r="T31" s="13"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32" s="37"/>
       <c r="H32" s="34"/>
       <c r="I32" s="4">
@@ -1637,7 +1652,7 @@
       </c>
       <c r="T32" s="13"/>
     </row>
-    <row r="33" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H33" s="37"/>
       <c r="R33" s="37"/>
     </row>
@@ -1647,12 +1662,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1800,15 +1812,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1832,10 +1848,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Täytettiin vaatimusmäärittelyä sekä lisättiin tulost-optio tulosten tarkasteluun -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAF61B8-CA7D-478D-AEA1-A147AFB731C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56080C27-A886-4CA3-92BE-43CBA9337B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>xaml, kaikenlaista hienosäätöä</t>
+  </si>
+  <si>
+    <t>Ohjelmiston demotus valmistelu</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -477,7 +480,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -775,38 +778,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="49.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="10" max="10" width="52.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" customWidth="1"/>
+    <col min="15" max="15" width="49.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="25.109375" customWidth="1"/>
     <col min="20" max="20" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
@@ -844,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
@@ -894,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="31">
         <v>45321</v>
       </c>
@@ -932,7 +935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="32">
         <v>45323</v>
       </c>
@@ -970,7 +973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="32">
         <v>45327</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="32">
         <v>45328</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="32">
         <v>45331</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="32">
         <v>45334</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="32">
         <v>45336</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="32" t="s">
         <v>19</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="32" t="s">
         <v>26</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="32">
         <v>45339</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="32">
         <v>45343</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="32">
         <v>45344</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="32">
         <v>45345</v>
       </c>
@@ -1388,7 +1391,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="32">
         <v>45347</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>45351</v>
       </c>
       <c r="N17" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O17" s="20" t="s">
         <v>42</v>
@@ -1426,7 +1429,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="32">
         <v>45348</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>45352</v>
       </c>
       <c r="N18" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O18" s="20" t="s">
         <v>46</v>
@@ -1464,7 +1467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="32">
         <v>45352</v>
       </c>
@@ -1483,9 +1486,15 @@
       <c r="J19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M19" s="34"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="12"/>
+      <c r="M19" s="34">
+        <v>45355</v>
+      </c>
+      <c r="N19" s="6">
+        <v>1</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="R19" s="35">
         <v>45347</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="32"/>
       <c r="D20" s="4"/>
       <c r="E20" s="12"/>
@@ -1522,7 +1531,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="32"/>
       <c r="D21" s="4"/>
       <c r="E21" s="12"/>
@@ -1542,7 +1551,7 @@
       <c r="S21" s="8"/>
       <c r="T21" s="12"/>
     </row>
-    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="32"/>
       <c r="D22" s="4"/>
       <c r="E22" s="12"/>
@@ -1556,7 +1565,7 @@
       <c r="S22" s="8"/>
       <c r="T22" s="12"/>
     </row>
-    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="32"/>
       <c r="D23" s="4"/>
       <c r="E23" s="12"/>
@@ -1570,7 +1579,7 @@
       <c r="S23" s="8"/>
       <c r="T23" s="12"/>
     </row>
-    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="32"/>
       <c r="D24" s="4"/>
       <c r="E24" s="12"/>
@@ -1584,7 +1593,7 @@
       <c r="S24" s="8"/>
       <c r="T24" s="12"/>
     </row>
-    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="32"/>
       <c r="D25" s="4"/>
       <c r="E25" s="12"/>
@@ -1598,7 +1607,7 @@
       <c r="S25" s="8"/>
       <c r="T25" s="12"/>
     </row>
-    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="32"/>
       <c r="D26" s="4"/>
       <c r="E26" s="12"/>
@@ -1612,7 +1621,7 @@
       <c r="S26" s="8"/>
       <c r="T26" s="12"/>
     </row>
-    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="32"/>
       <c r="D27" s="4"/>
       <c r="E27" s="12"/>
@@ -1626,7 +1635,7 @@
       <c r="S27" s="8"/>
       <c r="T27" s="12"/>
     </row>
-    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="32"/>
       <c r="D28" s="4"/>
       <c r="E28" s="12"/>
@@ -1640,7 +1649,7 @@
       <c r="S28" s="8"/>
       <c r="T28" s="12"/>
     </row>
-    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="32"/>
       <c r="D29" s="4"/>
       <c r="E29" s="12"/>
@@ -1654,7 +1663,7 @@
       <c r="S29" s="8"/>
       <c r="T29" s="12"/>
     </row>
-    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="32"/>
       <c r="D30" s="4"/>
       <c r="E30" s="12"/>
@@ -1668,7 +1677,7 @@
       <c r="S30" s="8"/>
       <c r="T30" s="12"/>
     </row>
-    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="C31" s="32"/>
       <c r="D31" s="4"/>
@@ -1683,7 +1692,7 @@
       <c r="S31" s="8"/>
       <c r="T31" s="12"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C32" s="39" t="s">
         <v>47</v>
       </c>
@@ -1705,7 +1714,7 @@
       </c>
       <c r="N32" s="7">
         <f>SUM(N3:N30)</f>
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O32" s="12"/>
       <c r="R32" s="41" t="s">
@@ -1717,7 +1726,7 @@
       </c>
       <c r="T32" s="12"/>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C33" s="36"/>
       <c r="H33" s="36"/>
       <c r="R33" s="36"/>
@@ -1729,12 +1738,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1882,15 +1888,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1914,10 +1924,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Korjattiin ohjelmistoa ja lisättiin tulostus -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56080C27-A886-4CA3-92BE-43CBA9337B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38696DF-2A4D-4432-8561-901BA72C27E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
@@ -185,7 +185,7 @@
     <t>xaml, kaikenlaista hienosäätöä</t>
   </si>
   <si>
-    <t>Ohjelmiston demotus valmistelu</t>
+    <t>Ohjelmiston kehitys, printtausnappi, ongelmien selvitys</t>
   </si>
 </sst>
 </file>
@@ -1738,9 +1738,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1888,19 +1891,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1924,9 +1923,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Korjattiin nappien skaalautuminen ampumataulukossa -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCD82F2-6BF2-4D97-B8C2-2C18528E9B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296D23BE-D3A1-4877-95E8-0961EEC33C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">Vaatimusmäärittelyn tekemistä </t>
   </si>
   <si>
-    <t>Esittely, ohjelmistonkehitys</t>
+    <t>Esittely, ohjelmiston kehitys</t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1537,9 +1537,9 @@
         <v>45721</v>
       </c>
       <c r="N20" s="6">
-        <v>2</v>
-      </c>
-      <c r="O20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="20" t="s">
         <v>52</v>
       </c>
       <c r="R20" s="35">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="M21" s="34"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="12"/>
+      <c r="O21" s="20"/>
       <c r="R21" s="35">
         <v>45355</v>
       </c>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="N32" s="7">
         <f>SUM(N3:N30)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O32" s="12"/>
       <c r="R32" s="41" t="s">
@@ -1771,12 +1771,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1924,15 +1921,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1956,10 +1957,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Teeman teko + ajankäyttö -IK
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eve\Documents\Hamk\ohjelmistoprojekti\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF135D-D986-4A4B-BCF0-84AAE450120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EACB86-EDDB-4F02-88D6-1E6219F88DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Hienosäätöä, esityksen suunnittelua</t>
+  </si>
+  <si>
+    <t>Teemat, opettelu ja tekeminen</t>
   </si>
 </sst>
 </file>
@@ -781,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +804,7 @@
     <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="49.5703125" customWidth="1"/>
+    <col min="15" max="15" width="53.7109375" customWidth="1"/>
     <col min="18" max="18" width="12.7109375" customWidth="1"/>
     <col min="19" max="19" width="25.140625" customWidth="1"/>
     <col min="20" max="20" width="68" customWidth="1"/>
@@ -1564,9 +1567,15 @@
       <c r="C22" s="32"/>
       <c r="D22" s="4"/>
       <c r="E22" s="12"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="12"/>
+      <c r="H22" s="33">
+        <v>45357</v>
+      </c>
+      <c r="I22" s="2">
+        <v>6</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="M22" s="34"/>
       <c r="N22" s="6"/>
       <c r="O22" s="12"/>
@@ -1715,7 +1724,7 @@
       </c>
       <c r="I32" s="3">
         <f>SUM(I3:I30)</f>
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="J32" s="12"/>
       <c r="M32" s="40" t="s">

</xml_diff>

<commit_message>
Korjattiin ja paikkailtiin ohjelmaa -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EACB86-EDDB-4F02-88D6-1E6219F88DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7BC17-8ACF-4252-8D9D-9D3C1C2B7376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Teemat, opettelu ja tekeminen</t>
+  </si>
+  <si>
+    <t>Ohjelmiston kehitys, taulukko, printtaus sekä esittäminen</t>
+  </si>
+  <si>
+    <t>Ohjelmiston kehity, merge ongelman setviminen</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,7 +492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -784,38 +790,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="53.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="10" max="10" width="52.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" customWidth="1"/>
+    <col min="15" max="15" width="53.6640625" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="25.109375" customWidth="1"/>
     <col min="20" max="20" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
@@ -853,7 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
@@ -903,7 +909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="31">
         <v>45321</v>
       </c>
@@ -941,7 +947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="32">
         <v>45323</v>
       </c>
@@ -979,7 +985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="32">
         <v>45327</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="32">
         <v>45328</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="32">
         <v>45331</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="32">
         <v>45334</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="32">
         <v>45336</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="32" t="s">
         <v>19</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="32" t="s">
         <v>26</v>
       </c>
@@ -1245,7 +1251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="32">
         <v>45339</v>
       </c>
@@ -1283,7 +1289,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="32">
         <v>45343</v>
       </c>
@@ -1321,7 +1327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="32">
         <v>45344</v>
       </c>
@@ -1359,7 +1365,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="32">
         <v>45345</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="32">
         <v>45347</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="32">
         <v>45348</v>
       </c>
@@ -1473,7 +1479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="32">
         <v>45352</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="32">
         <v>45355</v>
       </c>
@@ -1530,9 +1536,15 @@
       <c r="J20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="M20" s="34"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="12"/>
+      <c r="M20" s="34">
+        <v>45356</v>
+      </c>
+      <c r="N20" s="6">
+        <v>3</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="R20" s="35">
         <v>45352</v>
       </c>
@@ -1543,7 +1555,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="32"/>
       <c r="D21" s="4"/>
       <c r="E21" s="12"/>
@@ -1556,14 +1568,20 @@
       <c r="J21" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="34"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="12"/>
+      <c r="M21" s="34">
+        <v>45357</v>
+      </c>
+      <c r="N21" s="6">
+        <v>2</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="R21" s="35"/>
       <c r="S21" s="8"/>
       <c r="T21" s="12"/>
     </row>
-    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="32"/>
       <c r="D22" s="4"/>
       <c r="E22" s="12"/>
@@ -1583,7 +1601,7 @@
       <c r="S22" s="8"/>
       <c r="T22" s="12"/>
     </row>
-    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="32"/>
       <c r="D23" s="4"/>
       <c r="E23" s="12"/>
@@ -1597,7 +1615,7 @@
       <c r="S23" s="8"/>
       <c r="T23" s="12"/>
     </row>
-    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="32"/>
       <c r="D24" s="4"/>
       <c r="E24" s="12"/>
@@ -1611,7 +1629,7 @@
       <c r="S24" s="8"/>
       <c r="T24" s="12"/>
     </row>
-    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="32"/>
       <c r="D25" s="4"/>
       <c r="E25" s="12"/>
@@ -1625,7 +1643,7 @@
       <c r="S25" s="8"/>
       <c r="T25" s="12"/>
     </row>
-    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="32"/>
       <c r="D26" s="4"/>
       <c r="E26" s="12"/>
@@ -1639,7 +1657,7 @@
       <c r="S26" s="8"/>
       <c r="T26" s="12"/>
     </row>
-    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="32"/>
       <c r="D27" s="4"/>
       <c r="E27" s="12"/>
@@ -1653,7 +1671,7 @@
       <c r="S27" s="8"/>
       <c r="T27" s="12"/>
     </row>
-    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="32"/>
       <c r="D28" s="4"/>
       <c r="E28" s="12"/>
@@ -1667,7 +1685,7 @@
       <c r="S28" s="8"/>
       <c r="T28" s="12"/>
     </row>
-    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="32"/>
       <c r="D29" s="4"/>
       <c r="E29" s="12"/>
@@ -1681,7 +1699,7 @@
       <c r="S29" s="8"/>
       <c r="T29" s="12"/>
     </row>
-    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="32"/>
       <c r="D30" s="4"/>
       <c r="E30" s="12"/>
@@ -1695,7 +1713,7 @@
       <c r="S30" s="8"/>
       <c r="T30" s="12"/>
     </row>
-    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="C31" s="32"/>
       <c r="D31" s="4"/>
@@ -1710,7 +1728,7 @@
       <c r="S31" s="8"/>
       <c r="T31" s="12"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C32" s="39" t="s">
         <v>47</v>
       </c>
@@ -1732,7 +1750,7 @@
       </c>
       <c r="N32" s="7">
         <f>SUM(N3:N30)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="O32" s="12"/>
       <c r="R32" s="41" t="s">
@@ -1744,7 +1762,7 @@
       </c>
       <c r="T32" s="12"/>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C33" s="36"/>
       <c r="H33" s="36"/>
       <c r="R33" s="36"/>

</xml_diff>

<commit_message>
Lisättiin poistotoiminto sekä hienosäädettiin aikaa -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7BC17-8ACF-4252-8D9D-9D3C1C2B7376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EEF970-6F63-4F10-A021-58E799288853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
@@ -197,7 +197,7 @@
     <t>Ohjelmiston kehitys, taulukko, printtaus sekä esittäminen</t>
   </si>
   <si>
-    <t>Ohjelmiston kehity, merge ongelman setviminen</t>
+    <t>Ohjelmisto: merge selvitys, poistotoiminto, asettelutyö</t>
   </si>
 </sst>
 </file>
@@ -791,7 +791,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1572,9 +1572,9 @@
         <v>45357</v>
       </c>
       <c r="N21" s="6">
-        <v>2</v>
-      </c>
-      <c r="O21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="20" t="s">
         <v>53</v>
       </c>
       <c r="R21" s="35"/>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="N32" s="7">
         <f>SUM(N3:N30)</f>
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O32" s="12"/>
       <c r="R32" s="41" t="s">
@@ -1774,12 +1774,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1927,15 +1924,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1959,10 +1960,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Retron kirjaukset ja ajankäytönseuranta -IK
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AFA700-B25E-4439-A1D2-0B3C0111CBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB25102E-8A1A-4B33-8A57-40DED0AC239F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Ohjelmisto: merge selvitys, poistotoiminto, asettelutyö</t>
   </si>
   <si>
-    <t>Ohjelmistokehitys, skaalaus</t>
-  </si>
-  <si>
     <t>Json ja .gitignoren ja solmuun mennen ohjelman korjailua</t>
   </si>
   <si>
@@ -207,6 +204,24 @@
   </si>
   <si>
     <t>Katja Venäläinen</t>
+  </si>
+  <si>
+    <t>Esittely</t>
+  </si>
+  <si>
+    <t>Esittely ja vaatimusmäärittely</t>
+  </si>
+  <si>
+    <t>Vaatimusmäärittely</t>
+  </si>
+  <si>
+    <t>Ohjelmistokehitys, skaalaus, Retro, UML</t>
+  </si>
+  <si>
+    <t>Vaatimusmäärittely, Retro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Retro</t>
   </si>
 </sst>
 </file>
@@ -800,7 +815,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +834,7 @@
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="53.7109375" customWidth="1"/>
+    <col min="15" max="15" width="59.7109375" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
     <col min="18" max="18" width="12.7109375" customWidth="1"/>
     <col min="19" max="19" width="25.140625" customWidth="1"/>
@@ -871,7 +886,7 @@
     </row>
     <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="31">
         <v>45314</v>
@@ -883,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="26">
         <v>45314</v>
@@ -895,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M3" s="25">
         <v>45314</v>
@@ -907,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="Q3" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R3" s="29">
         <v>45314</v>
@@ -1566,9 +1581,15 @@
       </c>
     </row>
     <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="32"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="12"/>
+      <c r="C21" s="32">
+        <v>45356</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="H21" s="33">
         <v>45353</v>
       </c>
@@ -1587,14 +1608,26 @@
       <c r="O21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="R21" s="35"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="12"/>
+      <c r="R21" s="35">
+        <v>45354</v>
+      </c>
+      <c r="S21" s="8">
+        <v>2</v>
+      </c>
+      <c r="T21" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="32"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="12"/>
+      <c r="C22" s="32">
+        <v>45358</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="H22" s="33">
         <v>45356</v>
       </c>
@@ -1608,14 +1641,20 @@
         <v>45358</v>
       </c>
       <c r="N22" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O22" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="R22" s="35"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="R22" s="35">
+        <v>45356</v>
+      </c>
+      <c r="S22" s="8">
+        <v>3</v>
+      </c>
+      <c r="T22" s="20" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="32"/>
@@ -1627,23 +1666,35 @@
       <c r="I23" s="2">
         <v>6</v>
       </c>
-      <c r="J23" s="12" t="s">
-        <v>51</v>
+      <c r="J23" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="M23" s="34"/>
       <c r="N23" s="6"/>
       <c r="O23" s="12"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="12"/>
+      <c r="R23" s="35">
+        <v>45358</v>
+      </c>
+      <c r="S23" s="8">
+        <v>5</v>
+      </c>
+      <c r="T23" s="20" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="32"/>
       <c r="D24" s="4"/>
       <c r="E24" s="12"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="12"/>
+      <c r="H24" s="33">
+        <v>45358</v>
+      </c>
+      <c r="I24" s="2">
+        <v>4</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="M24" s="34"/>
       <c r="N24" s="6"/>
       <c r="O24" s="12"/>
@@ -1667,7 +1718,7 @@
     </row>
     <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="4"/>
@@ -1759,7 +1810,7 @@
       </c>
       <c r="D32" s="5">
         <f>SUM(D3:D31)</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E32" s="12"/>
       <c r="H32" s="38" t="s">
@@ -1767,7 +1818,7 @@
       </c>
       <c r="I32" s="3">
         <f>SUM(I3:I30)</f>
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J32" s="12"/>
       <c r="M32" s="40" t="s">
@@ -1775,7 +1826,7 @@
       </c>
       <c r="N32" s="7">
         <f>SUM(N3:N30)</f>
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="O32" s="12"/>
       <c r="R32" s="41" t="s">
@@ -1783,7 +1834,7 @@
       </c>
       <c r="S32" s="9">
         <f>SUM(S3:S30)</f>
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="T32" s="12"/>
     </row>
@@ -1799,9 +1850,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1949,19 +2003,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1985,9 +2035,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Hiottiin tulostusta ja tallennusta -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAD3113-946C-4E16-9289-3B7DCD050E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC4C8F5-3677-4A01-8599-0776865F1832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -215,13 +215,13 @@
     <t>Vaatimusmäärittely</t>
   </si>
   <si>
-    <t>Ohjelmistokehitys, skaalaus, Retro, UML</t>
-  </si>
-  <si>
     <t>Vaatimusmäärittely, Retro</t>
   </si>
   <si>
     <t xml:space="preserve"> Retro</t>
+  </si>
+  <si>
+    <t>Ohjelmistokehitys, skaalaus, Retro, UML, tulostus, yleinen hionta</t>
   </si>
 </sst>
 </file>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" topLeftCell="J11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1626,7 +1626,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H22" s="33">
         <v>45356</v>
@@ -1641,10 +1641,10 @@
         <v>45358</v>
       </c>
       <c r="N22" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O22" s="20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="R22" s="35">
         <v>45356</v>
@@ -1679,7 +1679,7 @@
         <v>6</v>
       </c>
       <c r="T23" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1693,7 +1693,7 @@
         <v>5</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M24" s="34"/>
       <c r="N24" s="6"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="N32" s="7">
         <f>SUM(N3:N30)</f>
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O32" s="12"/>
       <c r="R32" s="41" t="s">
@@ -1850,9 +1850,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2000,19 +2003,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2036,9 +2035,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Hienosäädettiin koodia ja päivitettiin UML-kuvaaja -JL
</commit_message>
<xml_diff>
--- a/Ajankäytönseurantagit.xlsx
+++ b/Ajankäytönseurantagit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eve\Documents\Hamk\ohjelmistoprojekti\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmistokehitys\Jiskan Gitit\AmpuminenR1\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAAA9D2-7132-4308-BD3F-FF394F68392E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392672A9-5638-4497-B0AC-DE2B223B28F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Vaatimusmäärittelyn viimeistely.</t>
+  </si>
+  <si>
+    <t>Ohjelmiston viilaamista, UML-kuvaajan päivitys</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,7 +525,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -820,39 +823,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="59.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="59.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="10" max="10" width="59.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" customWidth="1"/>
+    <col min="15" max="15" width="59.6640625" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="25.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="25.109375" customWidth="1"/>
     <col min="20" max="20" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
@@ -890,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21" t="s">
         <v>52</v>
       </c>
@@ -940,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="31">
         <v>45321</v>
       </c>
@@ -978,7 +981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="32">
         <v>45323</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="32">
         <v>45327</v>
       </c>
@@ -1054,7 +1057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="32">
         <v>45328</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="32">
         <v>45331</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="32">
         <v>45334</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="32">
         <v>45336</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="32" t="s">
         <v>15</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="32" t="s">
         <v>22</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="32">
         <v>45339</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="32">
         <v>45343</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="32">
         <v>45344</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="32">
         <v>45345</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="32">
         <v>45347</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="32">
         <v>45348</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="32">
         <v>45352</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="32">
         <v>45355</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="32">
         <v>45356</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="32">
         <v>45358</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="32">
         <v>45359</v>
       </c>
@@ -1681,9 +1684,15 @@
       <c r="J23" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="34"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="12"/>
+      <c r="M23" s="34">
+        <v>45360</v>
+      </c>
+      <c r="N23" s="6">
+        <v>2</v>
+      </c>
+      <c r="O23" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="R23" s="35">
         <v>45358</v>
       </c>
@@ -1694,7 +1703,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="32"/>
       <c r="D24" s="4"/>
       <c r="E24" s="12"/>
@@ -1714,7 +1723,7 @@
       <c r="S24" s="8"/>
       <c r="T24" s="12"/>
     </row>
-    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="32"/>
       <c r="D25" s="4"/>
       <c r="E25" s="12"/>
@@ -1734,7 +1743,7 @@
       <c r="S25" s="8"/>
       <c r="T25" s="12"/>
     </row>
-    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1751,7 +1760,7 @@
       <c r="S26" s="8"/>
       <c r="T26" s="12"/>
     </row>
-    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="32"/>
       <c r="D27" s="4"/>
       <c r="E27" s="12"/>
@@ -1765,7 +1774,7 @@
       <c r="S27" s="8"/>
       <c r="T27" s="12"/>
     </row>
-    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="32"/>
       <c r="D28" s="4"/>
       <c r="E28" s="12"/>
@@ -1779,7 +1788,7 @@
       <c r="S28" s="8"/>
       <c r="T28" s="12"/>
     </row>
-    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="32"/>
       <c r="D29" s="4"/>
       <c r="E29" s="12"/>
@@ -1793,7 +1802,7 @@
       <c r="S29" s="8"/>
       <c r="T29" s="12"/>
     </row>
-    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="32"/>
       <c r="D30" s="4"/>
       <c r="E30" s="12"/>
@@ -1807,7 +1816,7 @@
       <c r="S30" s="8"/>
       <c r="T30" s="12"/>
     </row>
-    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="C31" s="32"/>
       <c r="D31" s="4"/>
@@ -1822,7 +1831,7 @@
       <c r="S31" s="8"/>
       <c r="T31" s="12"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C32" s="39" t="s">
         <v>43</v>
       </c>
@@ -1844,7 +1853,7 @@
       </c>
       <c r="N32" s="7">
         <f>SUM(N3:N30)</f>
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O32" s="12"/>
       <c r="R32" s="41" t="s">
@@ -1856,7 +1865,7 @@
       </c>
       <c r="T32" s="12"/>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C33" s="36"/>
       <c r="H33" s="36"/>
       <c r="R33" s="36"/>
@@ -1868,12 +1877,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2021,15 +2027,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2053,10 +2063,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>